<commit_message>
added logout and changed application URL
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>INT@12798</t>
+  </si>
+  <si>
+    <t>ghause000@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -69,7 +72,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -354,18 +357,18 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I14" sqref="H13:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>7829850103</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -374,8 +377,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>